<commit_message>
uloha_06: Načtení a vizualizace naměřených dat
</commit_message>
<xml_diff>
--- a/uloha_06/data_06/data_06.xlsx
+++ b/uloha_06/data_06/data_06.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t xml:space="preserve">střední výkon Ptsr [mW]</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t xml:space="preserve">opakovací frekvence f [kHz]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kalibrace pro fotodiodu [mV]</t>
   </si>
   <si>
     <t xml:space="preserve">Vzorek 1</t>
@@ -45,19 +48,13 @@
     <t xml:space="preserve">d [cm]</t>
   </si>
   <si>
-    <t xml:space="preserve">výkon [mW]</t>
+    <t xml:space="preserve">P [mW]</t>
   </si>
   <si>
-    <t xml:space="preserve">transmitance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kalibrace [mV]</t>
+    <t xml:space="preserve">T [%]</t>
   </si>
   <si>
     <t xml:space="preserve">U [mV]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
   </si>
 </sst>
 </file>
@@ -68,11 +65,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,6 +86,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,16 +151,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -222,7 +249,35 @@
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Vzorek 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -232,18 +287,18 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>wattmetr!$H$1:$H$2</c:f>
+              <c:f>wattmetr!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>výkon [mW]</c:v>
+                  <c:v>P [mW]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff420e"/>
+              <a:srgbClr val="800080"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
@@ -254,7 +309,7 @@
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
+                <a:srgbClr val="800080"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -285,61 +340,61 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>wattmetr!$F$3:$F$17</c:f>
+              <c:f>wattmetr!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>15</c:v>
-                </c:pt>
+                <c:ptCount val="16"/>
                 <c:pt idx="1">
-                  <c:v>15.5</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.3</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>25</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35</c:v>
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>wattmetr!$H$3:$H$17</c:f>
+              <c:f>wattmetr!$C$3:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -347,62 +402,90 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="11">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.5</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.5</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.5</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.5</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="25836480"/>
-        <c:axId val="56072889"/>
+        <c:axId val="77397953"/>
+        <c:axId val="11447462"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25836480"/>
+        <c:axId val="77397953"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>d[cm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -425,12 +508,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56072889"/>
+        <c:crossAx val="11447462"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56072889"/>
+        <c:axId val="11447462"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,6 +528,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>výkon[mW]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -467,7 +578,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25836480"/>
+        <c:crossAx val="77397953"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -520,7 +631,35 @@
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Vzorek 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -530,29 +669,29 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>fotodioda!$C$2</c:f>
+              <c:f>wattmetr!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>U [mV]</c:v>
+                  <c:v>P [mW]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="800080"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="diamond"/>
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="800080"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -583,142 +722,152 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>fotodioda!$B$3:$B$20</c:f>
+              <c:f>wattmetr!$G$2:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
                   <c:v>-1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>-0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>fotodioda!$C$3:$C$20</c:f>
+              <c:f>wattmetr!$H$2:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>290</c:v>
-                </c:pt>
+                <c:ptCount val="16"/>
                 <c:pt idx="1">
-                  <c:v>290</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>290</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>288</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>284</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>282</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>278</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>274</c:v>
+                  <c:v>9.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>272</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>268</c:v>
+                  <c:v>8.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>266</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>264</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>264</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>262</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>260</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>250</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52751628"/>
-        <c:axId val="87581738"/>
+        <c:axId val="76171875"/>
+        <c:axId val="14556608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52751628"/>
+        <c:axId val="76171875"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>d[cm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -741,12 +890,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87581738"/>
+        <c:crossAx val="14556608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87581738"/>
+        <c:axId val="14556608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,6 +910,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>výkon[mW]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -783,7 +960,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52751628"/>
+        <c:crossAx val="76171875"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -846,6 +1023,339 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>fotodioda!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>U [mV]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fotodioda!$B$3:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fotodioda!$C$3:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="5984337"/>
+        <c:axId val="15128768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="5984337"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15128768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="15128768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="5984337"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>fotodioda!$H$1:$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -879,11 +1389,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1022,17 +1537,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="77637429"/>
-        <c:axId val="57622283"/>
+        <c:axId val="36835534"/>
+        <c:axId val="71159973"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77637429"/>
+        <c:axId val="36835534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1049,17 +1564,21 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57622283"/>
+        <c:crossAx val="71159973"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57622283"/>
+        <c:axId val="71159973"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1593,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1091,14 +1610,18 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77637429"/>
+        <c:crossAx val="36835534"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1124,7 +1647,11 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -1148,16 +1675,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>234000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>375480</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>641520</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1165,12 +1692,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8909640" y="593640"/>
-        <a:ext cx="5759640" cy="3237120"/>
+        <a:off x="234000" y="3399840"/>
+        <a:ext cx="5762520" cy="3237120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>309960</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>70920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>382680</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>56880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6477840" y="3322080"/>
+        <a:ext cx="5762160" cy="3237120"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1190,18 +1747,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>65160</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvPr id="2" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="4205520"/>
-        <a:ext cx="5754600" cy="3237120"/>
+        <a:ext cx="5753880" cy="3236400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1220,18 +1777,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>227520</xdr:colOff>
+      <xdr:colOff>226800</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvPr id="3" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6665040" y="4410360"/>
-        <a:ext cx="5754600" cy="3237480"/>
+        <a:ext cx="5753880" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1355,40 +1912,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="K1:L1 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>2.3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>6.07</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -1410,563 +1975,563 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="1" sqref="K1:L1 J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">A3-16</f>
         <v>-1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <f aca="false">C3/'mereni parametru laseru'!$B$1</f>
-        <v>0.733333333333333</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="D3" s="4" t="n">
+        <f aca="false">(C3/'mereni parametru laseru'!$B$1)*100</f>
+        <v>73.3333333333333</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <f aca="false">F3-16</f>
         <v>-1</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="I3" s="2" t="n">
-        <f aca="false">H3/'mereni parametru laseru'!$B$1</f>
-        <v>0.733333333333333</v>
+      <c r="I3" s="4" t="n">
+        <f aca="false">(H3/'mereni parametru laseru'!$B$1)*100</f>
+        <v>73.3333333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <f aca="false">A4-16</f>
         <v>0</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <f aca="false">C4/'mereni parametru laseru'!$B$1</f>
-        <v>0.8</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="D4" s="4" t="n">
+        <f aca="false">(C4/'mereni parametru laseru'!$B$1)*100</f>
+        <v>80</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>15.5</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <f aca="false">F4-16</f>
         <v>-0.5</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>10.5</v>
       </c>
-      <c r="I4" s="2" t="n">
-        <f aca="false">H4/'mereni parametru laseru'!$B$1</f>
-        <v>0.7</v>
+      <c r="I4" s="4" t="n">
+        <f aca="false">(H4/'mereni parametru laseru'!$B$1)*100</f>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <f aca="false">A5-16</f>
         <v>1</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <f aca="false">C5/'mereni parametru laseru'!$B$1</f>
-        <v>0.766666666666667</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="D5" s="4" t="n">
+        <f aca="false">(C5/'mereni parametru laseru'!$B$1)*100</f>
+        <v>76.6666666666667</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <f aca="false">F5-16</f>
         <v>0</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>10.5</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <f aca="false">H5/'mereni parametru laseru'!$B$1</f>
-        <v>0.7</v>
+      <c r="I5" s="4" t="n">
+        <f aca="false">(H5/'mereni parametru laseru'!$B$1)*100</f>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <f aca="false">A6-16</f>
         <v>2</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <f aca="false">C6/'mereni parametru laseru'!$B$1</f>
-        <v>0.766666666666667</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="D6" s="4" t="n">
+        <f aca="false">(C6/'mereni parametru laseru'!$B$1)*100</f>
+        <v>76.6666666666667</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>16.5</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <f aca="false">F6-16</f>
         <v>0.5</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I6" s="2" t="n">
-        <f aca="false">H6/'mereni parametru laseru'!$B$1</f>
-        <v>0.666666666666667</v>
+      <c r="I6" s="4" t="n">
+        <f aca="false">(H6/'mereni parametru laseru'!$B$1)*100</f>
+        <v>66.6666666666667</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <f aca="false">A7-16</f>
         <v>3</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="n">
-        <f aca="false">C7/'mereni parametru laseru'!$B$1</f>
-        <v>0.733333333333333</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="D7" s="4" t="n">
+        <f aca="false">(C7/'mereni parametru laseru'!$B$1)*100</f>
+        <v>73.3333333333333</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <f aca="false">F7-16</f>
         <v>1</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I7" s="2" t="n">
-        <f aca="false">H7/'mereni parametru laseru'!$B$1</f>
-        <v>0.666666666666667</v>
+      <c r="I7" s="4" t="n">
+        <f aca="false">(H7/'mereni parametru laseru'!$B$1)*100</f>
+        <v>66.6666666666667</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <f aca="false">A8-16</f>
         <v>4</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <f aca="false">C8/'mereni parametru laseru'!$B$1</f>
-        <v>0.733333333333333</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="D8" s="4" t="n">
+        <f aca="false">(C8/'mereni parametru laseru'!$B$1)*100</f>
+        <v>73.3333333333333</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>17.3</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <f aca="false">F8-16</f>
         <v>1.3</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>9.5</v>
       </c>
-      <c r="I8" s="2" t="n">
-        <f aca="false">H8/'mereni parametru laseru'!$B$1</f>
-        <v>0.633333333333333</v>
+      <c r="I8" s="4" t="n">
+        <f aca="false">(H8/'mereni parametru laseru'!$B$1)*100</f>
+        <v>63.3333333333333</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <f aca="false">A9-16</f>
         <v>5</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>10.5</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <f aca="false">C9/'mereni parametru laseru'!$B$1</f>
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="0" t="n">
+      <c r="D9" s="4" t="n">
+        <f aca="false">(C9/'mereni parametru laseru'!$B$1)*100</f>
+        <v>70</v>
+      </c>
+      <c r="F9" s="1" t="n">
         <v>17.5</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <f aca="false">F9-16</f>
         <v>1.5</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>9.2</v>
       </c>
-      <c r="I9" s="2" t="n">
-        <f aca="false">H9/'mereni parametru laseru'!$B$1</f>
-        <v>0.613333333333333</v>
+      <c r="I9" s="4" t="n">
+        <f aca="false">(H9/'mereni parametru laseru'!$B$1)*100</f>
+        <v>61.3333333333333</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <f aca="false">A10-16</f>
         <v>7</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>10.5</v>
       </c>
-      <c r="D10" s="2" t="n">
-        <f aca="false">C10/'mereni parametru laseru'!$B$1</f>
-        <v>0.7</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="D10" s="4" t="n">
+        <f aca="false">(C10/'mereni parametru laseru'!$B$1)*100</f>
+        <v>70</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <f aca="false">F10-16</f>
         <v>2</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>9.1</v>
       </c>
-      <c r="I10" s="2" t="n">
-        <f aca="false">H10/'mereni parametru laseru'!$B$1</f>
-        <v>0.606666666666667</v>
+      <c r="I10" s="4" t="n">
+        <f aca="false">(H10/'mereni parametru laseru'!$B$1)*100</f>
+        <v>60.6666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <f aca="false">A11-16</f>
         <v>9</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>10.5</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <f aca="false">C11/'mereni parametru laseru'!$B$1</f>
-        <v>0.7</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="D11" s="4" t="n">
+        <f aca="false">(C11/'mereni parametru laseru'!$B$1)*100</f>
+        <v>70</v>
+      </c>
+      <c r="F11" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <f aca="false">F11-16</f>
         <v>3</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>8.8</v>
       </c>
-      <c r="I11" s="2" t="n">
-        <f aca="false">H11/'mereni parametru laseru'!$B$1</f>
-        <v>0.586666666666667</v>
+      <c r="I11" s="4" t="n">
+        <f aca="false">(H11/'mereni parametru laseru'!$B$1)*100</f>
+        <v>58.6666666666667</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <f aca="false">A12-16</f>
         <v>11</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>10.5</v>
       </c>
-      <c r="D12" s="2" t="n">
-        <f aca="false">C12/'mereni parametru laseru'!$B$1</f>
-        <v>0.7</v>
-      </c>
-      <c r="F12" s="0" t="n">
+      <c r="D12" s="4" t="n">
+        <f aca="false">(C12/'mereni parametru laseru'!$B$1)*100</f>
+        <v>70</v>
+      </c>
+      <c r="F12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <f aca="false">F12-16</f>
         <v>4</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="I12" s="2" t="n">
-        <f aca="false">H12/'mereni parametru laseru'!$B$1</f>
-        <v>0.566666666666667</v>
+      <c r="I12" s="4" t="n">
+        <f aca="false">(H12/'mereni parametru laseru'!$B$1)*100</f>
+        <v>56.6666666666667</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <f aca="false">A13-16</f>
         <v>14</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <f aca="false">C13/'mereni parametru laseru'!$B$1</f>
-        <v>0.666666666666667</v>
-      </c>
-      <c r="F13" s="0" t="n">
+      <c r="D13" s="4" t="n">
+        <f aca="false">(C13/'mereni parametru laseru'!$B$1)*100</f>
+        <v>66.6666666666667</v>
+      </c>
+      <c r="F13" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <f aca="false">F13-16</f>
         <v>5</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <f aca="false">H13/'mereni parametru laseru'!$B$1</f>
-        <v>0.566666666666667</v>
+      <c r="I13" s="4" t="n">
+        <f aca="false">(H13/'mereni parametru laseru'!$B$1)*100</f>
+        <v>56.6666666666667</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <f aca="false">A14-16</f>
         <v>19</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="n">
-        <f aca="false">C14/'mereni parametru laseru'!$B$1</f>
-        <v>0.666666666666667</v>
-      </c>
-      <c r="F14" s="0" t="n">
+      <c r="D14" s="4" t="n">
+        <f aca="false">(C14/'mereni parametru laseru'!$B$1)*100</f>
+        <v>66.6666666666667</v>
+      </c>
+      <c r="F14" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <f aca="false">F14-16</f>
         <v>7</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="I14" s="2" t="n">
-        <f aca="false">H14/'mereni parametru laseru'!$B$1</f>
-        <v>0.566666666666667</v>
+      <c r="I14" s="4" t="n">
+        <f aca="false">(H14/'mereni parametru laseru'!$B$1)*100</f>
+        <v>56.6666666666667</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <f aca="false">A15-16</f>
         <v>24</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="D15" s="2" t="n">
-        <f aca="false">C15/'mereni parametru laseru'!$B$1</f>
-        <v>0.66</v>
-      </c>
-      <c r="F15" s="0" t="n">
+      <c r="D15" s="4" t="n">
+        <f aca="false">(C15/'mereni parametru laseru'!$B$1)*100</f>
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <f aca="false">F15-16</f>
         <v>9</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="I15" s="2" t="n">
-        <f aca="false">H15/'mereni parametru laseru'!$B$1</f>
-        <v>0.566666666666667</v>
+      <c r="I15" s="4" t="n">
+        <f aca="false">(H15/'mereni parametru laseru'!$B$1)*100</f>
+        <v>56.6666666666667</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <f aca="false">A16-16</f>
         <v>29</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="D16" s="2" t="n">
-        <f aca="false">C16/'mereni parametru laseru'!$B$1</f>
-        <v>0.66</v>
-      </c>
-      <c r="F16" s="0" t="n">
+      <c r="D16" s="4" t="n">
+        <f aca="false">(C16/'mereni parametru laseru'!$B$1)*100</f>
+        <v>66</v>
+      </c>
+      <c r="F16" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <f aca="false">F16-16</f>
         <v>14</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="I16" s="2" t="n">
-        <f aca="false">H16/'mereni parametru laseru'!$B$1</f>
-        <v>0.566666666666667</v>
+      <c r="I16" s="4" t="n">
+        <f aca="false">(H16/'mereni parametru laseru'!$B$1)*100</f>
+        <v>56.6666666666667</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <f aca="false">A17-16</f>
         <v>34</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="D17" s="2" t="n">
-        <f aca="false">C17/'mereni parametru laseru'!$B$1</f>
-        <v>0.66</v>
-      </c>
-      <c r="F17" s="0" t="n">
+      <c r="D17" s="4" t="n">
+        <f aca="false">(C17/'mereni parametru laseru'!$B$1)*100</f>
+        <v>66</v>
+      </c>
+      <c r="F17" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <f aca="false">F17-16</f>
         <v>19</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <f aca="false">H17/'mereni parametru laseru'!$B$1</f>
-        <v>0.566666666666667</v>
+      <c r="I17" s="4" t="n">
+        <f aca="false">(H17/'mereni parametru laseru'!$B$1)*100</f>
+        <v>56.6666666666667</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="D19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="D20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="D21" s="4"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="2"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="2"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="2"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="2"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="2"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="2"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="2"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="2"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="2"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="2"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="2"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="2"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="2"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="2"/>
+      <c r="D35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1992,627 +2557,623 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="K1" s="0" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="0" t="n">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>11</v>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">A3-16</f>
         <v>-1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <f aca="false">C3/348</f>
-        <v>0.833333333333333</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="D3" s="4" t="n">
+        <f aca="false">(C3/'mereni parametru laseru'!$B$4)*100</f>
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <f aca="false">F3-16</f>
         <v>-1</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>252</v>
       </c>
-      <c r="I3" s="2" t="n">
-        <f aca="false">H3/348</f>
-        <v>0.724137931034483</v>
+      <c r="I3" s="4" t="n">
+        <f aca="false">(H3/'mereni parametru laseru'!$B$4)*100</f>
+        <v>72.4137931034483</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>15.5</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <f aca="false">A4-16</f>
         <v>-0.5</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <f aca="false">C4/348</f>
-        <v>0.833333333333333</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="D4" s="4" t="n">
+        <f aca="false">(C4/'mereni parametru laseru'!$B$4)*100</f>
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>15.5</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <f aca="false">F4-16</f>
         <v>-0.5</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="I4" s="2" t="n">
-        <f aca="false">H4/348</f>
-        <v>0.718390804597701</v>
+      <c r="I4" s="4" t="n">
+        <f aca="false">(H4/'mereni parametru laseru'!$B$4)*100</f>
+        <v>71.8390804597701</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <f aca="false">A5-16</f>
         <v>0</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <f aca="false">C5/348</f>
-        <v>0.833333333333333</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="D5" s="4" t="n">
+        <f aca="false">(C5/'mereni parametru laseru'!$B$4)*100</f>
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>15.8</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <f aca="false">F5-16</f>
         <v>-0.199999999999999</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>248</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <f aca="false">H5/348</f>
-        <v>0.71264367816092</v>
+      <c r="I5" s="4" t="n">
+        <f aca="false">(H5/'mereni parametru laseru'!$B$4)*100</f>
+        <v>71.264367816092</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>16.5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <f aca="false">A6-16</f>
         <v>0.5</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>288</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <f aca="false">C6/348</f>
-        <v>0.827586206896552</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="D6" s="4" t="n">
+        <f aca="false">(C6/'mereni parametru laseru'!$B$4)*100</f>
+        <v>82.7586206896552</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <f aca="false">F6-16</f>
         <v>0</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>244</v>
       </c>
-      <c r="I6" s="2" t="n">
-        <f aca="false">H6/348</f>
-        <v>0.701149425287356</v>
+      <c r="I6" s="4" t="n">
+        <f aca="false">(H6/'mereni parametru laseru'!$B$4)*100</f>
+        <v>70.1149425287356</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <f aca="false">A7-16</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>284</v>
       </c>
-      <c r="D7" s="2" t="n">
-        <f aca="false">C7/348</f>
-        <v>0.816091954022989</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="D7" s="4" t="n">
+        <f aca="false">(C7/'mereni parametru laseru'!$B$4)*100</f>
+        <v>81.6091954022989</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>16.5</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <f aca="false">F7-16</f>
         <v>0.5</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>238</v>
       </c>
-      <c r="I7" s="2" t="n">
-        <f aca="false">H7/348</f>
-        <v>0.683908045977012</v>
+      <c r="I7" s="4" t="n">
+        <f aca="false">(H7/'mereni parametru laseru'!$B$4)*100</f>
+        <v>68.3908045977012</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>17.5</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <f aca="false">A8-16</f>
         <v>1.5</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>282</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <f aca="false">C8/348</f>
-        <v>0.810344827586207</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="D8" s="4" t="n">
+        <f aca="false">(C8/'mereni parametru laseru'!$B$4)*100</f>
+        <v>81.0344827586207</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <f aca="false">F8-16</f>
         <v>1</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>236</v>
       </c>
-      <c r="I8" s="2" t="n">
-        <f aca="false">H8/348</f>
-        <v>0.67816091954023</v>
+      <c r="I8" s="4" t="n">
+        <f aca="false">(H8/'mereni parametru laseru'!$B$4)*100</f>
+        <v>67.816091954023</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <f aca="false">A9-16</f>
         <v>2</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>278</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <f aca="false">C9/348</f>
-        <v>0.798850574712644</v>
-      </c>
-      <c r="F9" s="0" t="n">
+      <c r="D9" s="4" t="n">
+        <f aca="false">(C9/'mereni parametru laseru'!$B$4)*100</f>
+        <v>79.8850574712644</v>
+      </c>
+      <c r="F9" s="1" t="n">
         <v>17.5</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <f aca="false">F9-16</f>
         <v>1.5</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>234</v>
       </c>
-      <c r="I9" s="2" t="n">
-        <f aca="false">H9/348</f>
-        <v>0.672413793103448</v>
+      <c r="I9" s="4" t="n">
+        <f aca="false">(H9/'mereni parametru laseru'!$B$4)*100</f>
+        <v>67.2413793103448</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>18.5</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <f aca="false">A10-16</f>
         <v>2.5</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>274</v>
       </c>
-      <c r="D10" s="2" t="n">
-        <f aca="false">C10/348</f>
-        <v>0.78735632183908</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="D10" s="4" t="n">
+        <f aca="false">(C10/'mereni parametru laseru'!$B$4)*100</f>
+        <v>78.735632183908</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <f aca="false">F10-16</f>
         <v>2</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="I10" s="2" t="n">
-        <f aca="false">H10/348</f>
-        <v>0.666666666666667</v>
+      <c r="I10" s="4" t="n">
+        <f aca="false">(H10/'mereni parametru laseru'!$B$4)*100</f>
+        <v>66.6666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <f aca="false">A11-16</f>
         <v>3</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>272</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <f aca="false">C11/348</f>
-        <v>0.781609195402299</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="D11" s="4" t="n">
+        <f aca="false">(C11/'mereni parametru laseru'!$B$4)*100</f>
+        <v>78.1609195402299</v>
+      </c>
+      <c r="F11" s="1" t="n">
         <v>18.5</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <f aca="false">F11-16</f>
         <v>2.5</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="I11" s="2" t="n">
-        <f aca="false">H11/348</f>
-        <v>0.660919540229885</v>
+      <c r="I11" s="4" t="n">
+        <f aca="false">(H11/'mereni parametru laseru'!$B$4)*100</f>
+        <v>66.0919540229885</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <f aca="false">A12-16</f>
         <v>4</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>268</v>
       </c>
-      <c r="D12" s="2" t="n">
-        <f aca="false">C12/348</f>
-        <v>0.770114942528736</v>
-      </c>
-      <c r="F12" s="0" t="n">
+      <c r="D12" s="4" t="n">
+        <f aca="false">(C12/'mereni parametru laseru'!$B$4)*100</f>
+        <v>77.0114942528736</v>
+      </c>
+      <c r="F12" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <f aca="false">F12-16</f>
         <v>3</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>228</v>
       </c>
-      <c r="I12" s="2" t="n">
-        <f aca="false">H12/348</f>
-        <v>0.655172413793103</v>
+      <c r="I12" s="4" t="n">
+        <f aca="false">(H12/'mereni parametru laseru'!$B$4)*100</f>
+        <v>65.5172413793104</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <f aca="false">A13-16</f>
         <v>5</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>266</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <f aca="false">C13/348</f>
-        <v>0.764367816091954</v>
-      </c>
-      <c r="F13" s="0" t="n">
+      <c r="D13" s="4" t="n">
+        <f aca="false">(C13/'mereni parametru laseru'!$B$4)*100</f>
+        <v>76.4367816091954</v>
+      </c>
+      <c r="F13" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <f aca="false">F13-16</f>
         <v>4</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>228</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <f aca="false">H13/348</f>
-        <v>0.655172413793103</v>
+      <c r="I13" s="4" t="n">
+        <f aca="false">(H13/'mereni parametru laseru'!$B$4)*100</f>
+        <v>65.5172413793104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <f aca="false">A14-16</f>
         <v>7</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>264</v>
       </c>
-      <c r="D14" s="2" t="n">
-        <f aca="false">C14/348</f>
-        <v>0.758620689655172</v>
-      </c>
-      <c r="F14" s="0" t="n">
+      <c r="D14" s="4" t="n">
+        <f aca="false">(C14/'mereni parametru laseru'!$B$4)*100</f>
+        <v>75.8620689655172</v>
+      </c>
+      <c r="F14" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <f aca="false">F14-16</f>
         <v>5</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>224</v>
       </c>
-      <c r="I14" s="2" t="n">
-        <f aca="false">H14/348</f>
-        <v>0.64367816091954</v>
+      <c r="I14" s="4" t="n">
+        <f aca="false">(H14/'mereni parametru laseru'!$B$4)*100</f>
+        <v>64.367816091954</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <f aca="false">A15-16</f>
         <v>9</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>264</v>
       </c>
-      <c r="D15" s="2" t="n">
-        <f aca="false">C15/348</f>
-        <v>0.758620689655172</v>
-      </c>
-      <c r="F15" s="0" t="n">
+      <c r="D15" s="4" t="n">
+        <f aca="false">(C15/'mereni parametru laseru'!$B$4)*100</f>
+        <v>75.8620689655172</v>
+      </c>
+      <c r="F15" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <f aca="false">F15-16</f>
         <v>7</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="I15" s="2" t="n">
-        <f aca="false">H15/348</f>
-        <v>0.637931034482759</v>
+      <c r="I15" s="4" t="n">
+        <f aca="false">(H15/'mereni parametru laseru'!$B$4)*100</f>
+        <v>63.7931034482759</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <f aca="false">A16-16</f>
         <v>14</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>262</v>
       </c>
-      <c r="D16" s="2" t="n">
-        <f aca="false">C16/348</f>
-        <v>0.752873563218391</v>
-      </c>
-      <c r="F16" s="0" t="n">
+      <c r="D16" s="4" t="n">
+        <f aca="false">(C16/'mereni parametru laseru'!$B$4)*100</f>
+        <v>75.2873563218391</v>
+      </c>
+      <c r="F16" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <f aca="false">F16-16</f>
         <v>9</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="I16" s="2" t="n">
-        <f aca="false">H16/348</f>
-        <v>0.632183908045977</v>
+      <c r="I16" s="4" t="n">
+        <f aca="false">(H16/'mereni parametru laseru'!$B$4)*100</f>
+        <v>63.2183908045977</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <f aca="false">A17-16</f>
         <v>19</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>260</v>
       </c>
-      <c r="D17" s="2" t="n">
-        <f aca="false">C17/348</f>
-        <v>0.747126436781609</v>
-      </c>
-      <c r="F17" s="0" t="n">
+      <c r="D17" s="4" t="n">
+        <f aca="false">(C17/'mereni parametru laseru'!$B$4)*100</f>
+        <v>74.7126436781609</v>
+      </c>
+      <c r="F17" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <f aca="false">F17-16</f>
         <v>11</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>216</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <f aca="false">H17/348</f>
-        <v>0.620689655172414</v>
+      <c r="I17" s="4" t="n">
+        <f aca="false">(H17/'mereni parametru laseru'!$B$4)*100</f>
+        <v>62.0689655172414</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <f aca="false">A18-16</f>
         <v>24</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="D18" s="2" t="n">
-        <f aca="false">C18/348</f>
-        <v>0.735632183908046</v>
-      </c>
-      <c r="F18" s="0" t="n">
+      <c r="D18" s="4" t="n">
+        <f aca="false">(C18/'mereni parametru laseru'!$B$4)*100</f>
+        <v>73.5632183908046</v>
+      </c>
+      <c r="F18" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <f aca="false">F18-16</f>
         <v>14</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>214</v>
       </c>
-      <c r="I18" s="2" t="n">
-        <f aca="false">H18/348</f>
-        <v>0.614942528735632</v>
+      <c r="I18" s="4" t="n">
+        <f aca="false">(H18/'mereni parametru laseru'!$B$4)*100</f>
+        <v>61.4942528735632</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <f aca="false">A19-16</f>
         <v>29</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>252</v>
       </c>
-      <c r="D19" s="2" t="n">
-        <f aca="false">C19/348</f>
-        <v>0.724137931034483</v>
-      </c>
-      <c r="F19" s="0" t="n">
+      <c r="D19" s="4" t="n">
+        <f aca="false">(C19/'mereni parametru laseru'!$B$4)*100</f>
+        <v>72.4137931034483</v>
+      </c>
+      <c r="F19" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <f aca="false">F19-16</f>
         <v>19</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>210</v>
       </c>
-      <c r="I19" s="2" t="n">
-        <f aca="false">H19/348</f>
-        <v>0.603448275862069</v>
+      <c r="I19" s="4" t="n">
+        <f aca="false">(H19/'mereni parametru laseru'!$B$4)*100</f>
+        <v>60.3448275862069</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <f aca="false">A20-16</f>
         <v>34</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="D20" s="2" t="n">
-        <f aca="false">C20/348</f>
-        <v>0.718390804597701</v>
-      </c>
-      <c r="F20" s="0" t="n">
+      <c r="D20" s="4" t="n">
+        <f aca="false">(C20/'mereni parametru laseru'!$B$4)*100</f>
+        <v>71.8390804597701</v>
+      </c>
+      <c r="F20" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <f aca="false">F20-16</f>
         <v>24</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="I20" s="2" t="n">
-        <f aca="false">H20/348</f>
-        <v>0.597701149425287</v>
+      <c r="I20" s="4" t="n">
+        <f aca="false">(H20/'mereni parametru laseru'!$B$4)*100</f>
+        <v>59.7701149425287</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <f aca="false">F21-16</f>
         <v>29</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="I21" s="2" t="n">
-        <f aca="false">H21/348</f>
-        <v>0.597701149425287</v>
+      <c r="I21" s="4" t="n">
+        <f aca="false">(H21/'mereni parametru laseru'!$B$4)*100</f>
+        <v>59.7701149425287</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <f aca="false">F22-16</f>
         <v>34</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="I22" s="2" t="n">
-        <f aca="false">H22/348</f>
-        <v>0.597701149425287</v>
+      <c r="I22" s="4" t="n">
+        <f aca="false">(H22/'mereni parametru laseru'!$B$4)*100</f>
+        <v>59.7701149425287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uloha_06: Úkol 6, tabulky
</commit_message>
<xml_diff>
--- a/uloha_06/data_06/data_06.xlsx
+++ b/uloha_06/data_06/data_06.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="mereni parametru laseru" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="19">
   <si>
     <t>délka pulsu Tp [ns]</t>
   </si>
@@ -64,12 +64,33 @@
   <si>
     <t>\tabh{d}{cm}</t>
   </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\tabh{T}{%}</t>
+  </si>
+  <si>
+    <t>\\ \hline</t>
+  </si>
+  <si>
+    <t>Vzorek 1 -- wattmetr</t>
+  </si>
+  <si>
+    <t>Vzorek1 -- fotodioda</t>
+  </si>
+  <si>
+    <t>Vzorek 2 -- wattmetr</t>
+  </si>
+  <si>
+    <t>Vzorek2 -- fotodioda</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -80,6 +101,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,18 +128,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2042,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2621,7 +2657,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3257,199 +3293,974 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X32" sqref="X32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="M1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-1</v>
       </c>
-      <c r="C3">
-        <v>11</v>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3" s="5">
         <v>73.333333333333329</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="8">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3">
+        <v>-1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="5">
+        <v>73.333333333333329</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3">
+        <v>-1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="5">
+        <v>72.41379310344827</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="5">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>-0.5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="8">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4">
+        <v>-0.5</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="5">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4">
+        <v>-0.5</v>
+      </c>
+      <c r="T4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="5">
+        <v>71.839080459770116</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>11.5</v>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="5">
         <v>76.666666666666671</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="8">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="5">
+        <v>70</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5">
+        <v>-0.19999999999999929</v>
+      </c>
+      <c r="T5" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" s="5">
+        <v>71.264367816091962</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>11.5</v>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="5">
         <v>76.666666666666671</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="8">
+        <v>82.758620689655174</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="5">
+        <v>66.666666666666657</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U6" s="5">
+        <v>70.114942528735639</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>11</v>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
       <c r="D7" s="5">
         <v>73.333333333333329</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="8">
+        <v>81.609195402298852</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="5">
+        <v>66.666666666666657</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7">
+        <v>0.5</v>
+      </c>
+      <c r="T7" t="s">
+        <v>12</v>
+      </c>
+      <c r="U7" s="5">
+        <v>68.390804597701148</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>11</v>
+      <c r="C8" t="s">
+        <v>12</v>
       </c>
       <c r="D8" s="5">
         <v>73.333333333333329</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>1.5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8">
+        <v>81.034482758620683</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8">
+        <v>1.3000000000000007</v>
+      </c>
+      <c r="O8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="5">
+        <v>63.333333333333329</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="5">
+        <v>67.81609195402298</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9">
-        <v>10.5</v>
+      <c r="C9" t="s">
+        <v>12</v>
       </c>
       <c r="D9" s="5">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="8">
+        <v>79.885057471264361</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9">
+        <v>1.5</v>
+      </c>
+      <c r="O9" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="5">
+        <v>61.333333333333329</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9">
+        <v>1.5</v>
+      </c>
+      <c r="T9" t="s">
+        <v>12</v>
+      </c>
+      <c r="U9" s="5">
+        <v>67.241379310344826</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10">
-        <v>10.5</v>
+      <c r="C10" t="s">
+        <v>12</v>
       </c>
       <c r="D10" s="5">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>2.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="8">
+        <v>78.735632183908038</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="5">
+        <v>60.666666666666671</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="5">
+        <v>66.666666666666657</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>10.5</v>
+      <c r="C11" t="s">
+        <v>12</v>
       </c>
       <c r="D11" s="5">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="8">
+        <v>78.160919540229884</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="5">
+        <v>58.666666666666664</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S11">
+        <v>2.5</v>
+      </c>
+      <c r="T11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="5">
+        <v>66.091954022988503</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>10.5</v>
+      <c r="C12" t="s">
+        <v>12</v>
       </c>
       <c r="D12" s="5">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="8">
+        <v>77.011494252873561</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="5">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+      <c r="T12" t="s">
+        <v>12</v>
+      </c>
+      <c r="U12" s="5">
+        <v>65.517241379310349</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>14</v>
       </c>
-      <c r="C13">
-        <v>10</v>
+      <c r="C13" t="s">
+        <v>12</v>
       </c>
       <c r="D13" s="5">
         <v>66.666666666666657</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="8">
+        <v>76.436781609195407</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="5">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="5">
+        <v>65.517241379310349</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>19</v>
       </c>
-      <c r="C14">
-        <v>10</v>
+      <c r="C14" t="s">
+        <v>12</v>
       </c>
       <c r="D14" s="5">
         <v>66.666666666666657</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="8">
+        <v>75.862068965517238</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" s="5">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="T14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U14" s="5">
+        <v>64.367816091954026</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>24</v>
       </c>
-      <c r="C15">
-        <v>9.9</v>
+      <c r="C15" t="s">
+        <v>12</v>
       </c>
       <c r="D15" s="5">
         <v>66</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="8">
+        <v>75.862068965517238</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" s="5">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15">
+        <v>7</v>
+      </c>
+      <c r="T15" t="s">
+        <v>12</v>
+      </c>
+      <c r="U15" s="5">
+        <v>63.793103448275865</v>
+      </c>
+      <c r="V15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>29</v>
       </c>
-      <c r="C16">
-        <v>9.9</v>
+      <c r="C16" t="s">
+        <v>12</v>
       </c>
       <c r="D16" s="5">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="8">
+        <v>75.287356321839084</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="5">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S16">
+        <v>9</v>
+      </c>
+      <c r="T16" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="5">
+        <v>63.218390804597703</v>
+      </c>
+      <c r="V16" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>34</v>
       </c>
-      <c r="C17">
-        <v>9.9</v>
+      <c r="C17" t="s">
+        <v>12</v>
       </c>
       <c r="D17" s="5">
         <v>66</v>
       </c>
+      <c r="E17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="8">
+        <v>74.712643678160916</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17">
+        <v>19</v>
+      </c>
+      <c r="O17" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" s="5">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S17">
+        <v>11</v>
+      </c>
+      <c r="T17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17" s="5">
+        <v>62.068965517241381</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="8">
+        <v>73.563218390804593</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S18">
+        <v>14</v>
+      </c>
+      <c r="T18" t="s">
+        <v>12</v>
+      </c>
+      <c r="U18" s="5">
+        <v>61.494252873563212</v>
+      </c>
+      <c r="V18" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>29</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="8">
+        <v>72.41379310344827</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S19">
+        <v>19</v>
+      </c>
+      <c r="T19" t="s">
+        <v>12</v>
+      </c>
+      <c r="U19" s="5">
+        <v>60.344827586206897</v>
+      </c>
+      <c r="V19" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="8">
+        <v>71.839080459770116</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S20">
+        <v>24</v>
+      </c>
+      <c r="T20" t="s">
+        <v>12</v>
+      </c>
+      <c r="U20" s="5">
+        <v>59.770114942528743</v>
+      </c>
+      <c r="V20" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="S21">
+        <v>29</v>
+      </c>
+      <c r="T21" t="s">
+        <v>12</v>
+      </c>
+      <c r="U21" s="5">
+        <v>59.770114942528743</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="S22">
+        <v>34</v>
+      </c>
+      <c r="T22" t="s">
+        <v>12</v>
+      </c>
+      <c r="U22" s="5">
+        <v>59.770114942528743</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="\\"/>
+    <hyperlink ref="E3:E17" r:id="rId2" display="\\"/>
+    <hyperlink ref="J2" r:id="rId3" display="\\"/>
+    <hyperlink ref="J3:J20" r:id="rId4" display="\\"/>
+    <hyperlink ref="Q2" r:id="rId5" display="\\"/>
+    <hyperlink ref="V2" r:id="rId6" display="\\"/>
+    <hyperlink ref="Q3:Q17" r:id="rId7" display="\\"/>
+    <hyperlink ref="V3:V22" r:id="rId8" display="\\"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>